<commit_message>
code(US-Tool): move the length of geothermal probe to the us-sheet, since this is a location-dependent variable.
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C554C408-60E2-5D4B-BA44-4BA1797DF274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129BF5FB-302D-D04B-A26F-FD7329CBCC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34520" yWindow="0" windowWidth="34280" windowHeight="28800" activeTab="7" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="34520" yWindow="500" windowWidth="34280" windowHeight="26300" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="361">
   <si>
     <t>start date</t>
   </si>
@@ -653,9 +653,6 @@
   </si>
   <si>
     <t>quality grade</t>
-  </si>
-  <si>
-    <t>length of the geoth. probe</t>
   </si>
   <si>
     <t>heat extraction</t>
@@ -1753,7 +1750,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1768,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1805,7 +1802,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -1831,13 +1828,13 @@
         <v>105</v>
       </c>
       <c r="B1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" t="s">
         <v>280</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>281</v>
-      </c>
-      <c r="D1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3354,7 +3351,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B111">
         <v>0.35</v>
@@ -3368,7 +3365,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B112">
         <v>0.21</v>
@@ -3396,7 +3393,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B114">
         <v>7.14</v>
@@ -3424,7 +3421,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B116">
         <v>286</v>
@@ -3469,19 +3466,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>289</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>290</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>197</v>
@@ -3502,13 +3499,13 @@
         <v>153</v>
       </c>
       <c r="L1" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>292</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>293</v>
       </c>
       <c r="O1" t="s">
         <v>188</v>
@@ -3532,7 +3529,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B3" s="13">
         <v>0</v>
@@ -3565,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M3" s="13">
         <v>1</v>
@@ -3579,7 +3576,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B4" s="13">
         <v>0</v>
@@ -3612,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M4" s="13">
         <v>1</v>
@@ -3626,7 +3623,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B5" s="13">
         <v>0</v>
@@ -3659,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M5" s="13">
         <v>1</v>
@@ -3673,7 +3670,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
@@ -3706,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M6" s="13">
         <v>1</v>
@@ -3720,7 +3717,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -3753,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M7" s="13">
         <v>1</v>
@@ -3767,7 +3764,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
@@ -3800,7 +3797,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M8" s="13">
         <v>0</v>
@@ -3814,7 +3811,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
@@ -3847,7 +3844,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M9" s="13">
         <v>1</v>
@@ -3861,7 +3858,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B10" s="13">
         <v>0</v>
@@ -3894,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M10" s="13">
         <v>1</v>
@@ -3908,7 +3905,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11" s="13">
         <v>0</v>
@@ -3941,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M11" s="13">
         <v>1</v>
@@ -3955,7 +3952,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" s="13">
         <v>0</v>
@@ -3988,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M12" s="13">
         <v>1</v>
@@ -4002,7 +3999,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B13" s="13">
         <v>0</v>
@@ -4035,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M13" s="13">
         <v>1</v>
@@ -4049,7 +4046,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B14" s="13">
         <v>0</v>
@@ -4082,7 +4079,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M14" s="13">
         <v>1</v>
@@ -4096,7 +4093,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B15" s="13">
         <v>0</v>
@@ -4129,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M15" s="13">
         <v>1</v>
@@ -4143,7 +4140,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
@@ -4176,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M16" s="13">
         <v>1</v>
@@ -4190,7 +4187,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
@@ -4223,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M17" s="13">
         <v>1</v>
@@ -4237,7 +4234,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B18" s="13">
         <v>0</v>
@@ -4270,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M18" s="13">
         <v>1</v>
@@ -4284,7 +4281,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B19" s="13">
         <v>0</v>
@@ -4317,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M19" s="13">
         <v>1</v>
@@ -4331,7 +4328,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B20" s="13">
         <v>0</v>
@@ -4364,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M20" s="13">
         <v>1</v>
@@ -4378,7 +4375,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="13">
         <v>0</v>
@@ -4411,7 +4408,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M21" s="13">
         <v>1</v>
@@ -4425,7 +4422,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B22" s="13">
         <v>0</v>
@@ -4458,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M22" s="13">
         <v>1</v>
@@ -4472,7 +4469,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4505,7 +4502,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -4519,7 +4516,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4566,7 +4563,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4613,7 +4610,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4689,13 +4686,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>318</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>188</v>
@@ -4709,7 +4706,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B2" s="6">
         <v>0.15655827580000001</v>
@@ -4729,7 +4726,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B3" s="6">
         <v>85</v>
@@ -4749,7 +4746,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4811,7 +4808,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4840,7 +4837,7 @@
         <v>366</v>
       </c>
       <c r="I3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4869,7 +4866,7 @@
         <v>366</v>
       </c>
       <c r="I4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4898,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5072,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5101,7 +5098,7 @@
         <v>366</v>
       </c>
       <c r="I12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5188,7 +5185,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5217,7 +5214,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5246,7 +5243,7 @@
         <v>366</v>
       </c>
       <c r="I17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -5275,7 +5272,7 @@
         <v>366</v>
       </c>
       <c r="I18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -5304,7 +5301,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -5333,7 +5330,7 @@
         <v>436</v>
       </c>
       <c r="I20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -5362,7 +5359,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -5396,7 +5393,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5420,7 +5417,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -5478,7 +5475,7 @@
         <v>366</v>
       </c>
       <c r="I25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -5512,7 +5509,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -5536,7 +5533,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -5565,7 +5562,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -5623,7 +5620,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -5681,7 +5678,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -5802,7 +5799,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -5888,7 +5885,7 @@
         <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -5923,7 +5920,7 @@
         <v>0.9</v>
       </c>
       <c r="J3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -5955,7 +5952,7 @@
         <v>0.9</v>
       </c>
       <c r="J4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -5987,7 +5984,7 @@
         <v>0.9</v>
       </c>
       <c r="J5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -6019,7 +6016,7 @@
         <v>0.9</v>
       </c>
       <c r="J6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -6051,7 +6048,7 @@
         <v>0.9</v>
       </c>
       <c r="J7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -6083,7 +6080,7 @@
         <v>0.9</v>
       </c>
       <c r="J8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6115,7 +6112,7 @@
         <v>0.9</v>
       </c>
       <c r="J9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -6147,7 +6144,7 @@
         <v>0.9</v>
       </c>
       <c r="J10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -6179,7 +6176,7 @@
         <v>0.85</v>
       </c>
       <c r="J11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -6211,7 +6208,7 @@
         <v>0.85</v>
       </c>
       <c r="J12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -6243,7 +6240,7 @@
         <v>0.89</v>
       </c>
       <c r="J13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -6275,7 +6272,7 @@
         <v>0.89</v>
       </c>
       <c r="J14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -6307,7 +6304,7 @@
         <v>0.9</v>
       </c>
       <c r="J15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -6339,7 +6336,7 @@
         <v>0.9</v>
       </c>
       <c r="J16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -6371,7 +6368,7 @@
         <v>0.91</v>
       </c>
       <c r="J17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -6403,7 +6400,7 @@
         <v>0.91</v>
       </c>
       <c r="J18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -6435,7 +6432,7 @@
         <v>0.91</v>
       </c>
       <c r="J19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -6467,7 +6464,7 @@
         <v>0.91</v>
       </c>
       <c r="J20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -6499,7 +6496,7 @@
         <v>0.9</v>
       </c>
       <c r="J21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -6531,7 +6528,7 @@
         <v>0.9</v>
       </c>
       <c r="J22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -6563,7 +6560,7 @@
         <v>0.9</v>
       </c>
       <c r="J23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6595,7 +6592,7 @@
         <v>0.9</v>
       </c>
       <c r="J24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -6627,7 +6624,7 @@
         <v>0.9</v>
       </c>
       <c r="J25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -6659,7 +6656,7 @@
         <v>0.9</v>
       </c>
       <c r="J26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -6691,7 +6688,7 @@
         <v>0.85</v>
       </c>
       <c r="J27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -6723,7 +6720,7 @@
         <v>0.85</v>
       </c>
       <c r="J28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -6755,7 +6752,7 @@
         <v>0.91</v>
       </c>
       <c r="J29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -6787,7 +6784,7 @@
         <v>0.91</v>
       </c>
       <c r="J30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -6819,7 +6816,7 @@
         <v>0.91</v>
       </c>
       <c r="J31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -6851,7 +6848,7 @@
         <v>0.91</v>
       </c>
       <c r="J32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -6883,7 +6880,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -15965,7 +15962,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -16061,7 +16058,7 @@
         <v>196</v>
       </c>
       <c r="AG1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -16167,7 +16164,7 @@
         <v>0</v>
       </c>
       <c r="AG3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
@@ -16268,7 +16265,7 @@
         <v>0</v>
       </c>
       <c r="AG4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -16369,7 +16366,7 @@
         <v>0</v>
       </c>
       <c r="AG5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
@@ -16470,7 +16467,7 @@
         <v>0</v>
       </c>
       <c r="AG6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -16571,7 +16568,7 @@
         <v>0</v>
       </c>
       <c r="AG7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -16586,10 +16583,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
-  <dimension ref="A1:AQ25"/>
+  <dimension ref="A1:AP25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16600,15 +16597,15 @@
     <col min="12" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D1" t="s">
         <v>147</v>
@@ -16727,25 +16724,22 @@
       <c r="AP1" t="s">
         <v>219</v>
       </c>
-      <c r="AQ1" t="s">
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E3" t="s">
         <v>221</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D3" t="s">
-        <v>346</v>
-      </c>
-      <c r="E3" t="s">
-        <v>222</v>
       </c>
       <c r="F3">
         <v>0.375</v>
@@ -16858,25 +16852,22 @@
       <c r="AP3">
         <v>0</v>
       </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4">
         <v>0.39</v>
@@ -16989,25 +16980,22 @@
       <c r="AP4">
         <v>0</v>
       </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5">
         <v>0.92</v>
@@ -17120,25 +17108,22 @@
       <c r="AP5">
         <v>0</v>
       </c>
-      <c r="AQ5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D6" t="s">
+        <v>348</v>
+      </c>
+      <c r="E6" t="s">
         <v>225</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>340</v>
-      </c>
-      <c r="D6" t="s">
-        <v>349</v>
-      </c>
-      <c r="E6" t="s">
-        <v>226</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -17186,10 +17171,10 @@
         <v>0</v>
       </c>
       <c r="U6" t="s">
+        <v>226</v>
+      </c>
+      <c r="V6" t="s">
         <v>227</v>
-      </c>
-      <c r="V6" t="s">
-        <v>228</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -17198,13 +17183,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="Y6">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="Z6">
         <v>100</v>
       </c>
-      <c r="Z6">
-        <v>3.2800000000000003E-2</v>
-      </c>
       <c r="AA6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <v>0</v>
@@ -17251,25 +17236,22 @@
       <c r="AP6">
         <v>0</v>
       </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -17317,10 +17299,10 @@
         <v>0</v>
       </c>
       <c r="U7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -17335,13 +17317,13 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB7">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AC7">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -17382,25 +17364,22 @@
       <c r="AP7">
         <v>0</v>
       </c>
-      <c r="AQ7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -17448,10 +17427,10 @@
         <v>0</v>
       </c>
       <c r="U8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -17513,25 +17492,22 @@
       <c r="AP8">
         <v>0</v>
       </c>
-      <c r="AQ8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -17579,10 +17555,10 @@
         <v>0</v>
       </c>
       <c r="U9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -17597,13 +17573,13 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB9">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AC9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -17644,25 +17620,22 @@
       <c r="AP9">
         <v>0</v>
       </c>
-      <c r="AQ9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D10" t="s">
         <v>352</v>
       </c>
-      <c r="D10" t="s">
-        <v>353</v>
-      </c>
       <c r="E10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -17775,13 +17748,10 @@
       <c r="AP10">
         <v>0</v>
       </c>
-      <c r="AQ10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -17790,7 +17760,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F11">
         <v>0.78500000000000003</v>
@@ -17903,13 +17873,10 @@
       <c r="AP11">
         <v>0</v>
       </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -17918,7 +17885,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F12">
         <v>0.83</v>
@@ -18031,25 +17998,22 @@
       <c r="AP12">
         <v>0</v>
       </c>
-      <c r="AQ12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F13">
         <v>0.4</v>
@@ -18162,13 +18126,10 @@
       <c r="AP13">
         <v>0</v>
       </c>
-      <c r="AQ13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -18177,7 +18138,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F14">
         <v>0.98</v>
@@ -18290,13 +18251,10 @@
       <c r="AP14">
         <v>0</v>
       </c>
-      <c r="AQ14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -18305,7 +18263,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F15">
         <v>0.98</v>
@@ -18418,13 +18376,10 @@
       <c r="AP15">
         <v>0</v>
       </c>
-      <c r="AQ15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -18433,7 +18388,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F16">
         <v>0.98</v>
@@ -18546,25 +18501,22 @@
       <c r="AP16">
         <v>0</v>
       </c>
-      <c r="AQ16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F17">
         <v>0.92</v>
@@ -18677,25 +18629,22 @@
       <c r="AP17">
         <v>0</v>
       </c>
-      <c r="AQ17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -18743,10 +18692,10 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
+        <v>226</v>
+      </c>
+      <c r="V18" t="s">
         <v>227</v>
-      </c>
-      <c r="V18" t="s">
-        <v>228</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -18755,13 +18704,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="Y18">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="Z18">
         <v>100</v>
       </c>
-      <c r="Z18">
-        <v>3.2800000000000003E-2</v>
-      </c>
       <c r="AA18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AB18">
         <v>0</v>
@@ -18808,25 +18757,22 @@
       <c r="AP18">
         <v>0</v>
       </c>
-      <c r="AQ18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F19">
         <v>0.35</v>
@@ -18939,25 +18885,22 @@
       <c r="AP19">
         <v>0</v>
       </c>
-      <c r="AQ19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F20">
         <v>0.35</v>
@@ -19070,25 +19013,22 @@
       <c r="AP20">
         <v>0</v>
       </c>
-      <c r="AQ20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D21" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F21">
         <v>0.92</v>
@@ -19201,25 +19141,22 @@
       <c r="AP21">
         <v>0</v>
       </c>
-      <c r="AQ21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F22">
         <v>0.9</v>
@@ -19332,25 +19269,22 @@
       <c r="AP22">
         <v>0</v>
       </c>
-      <c r="AQ22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F23">
         <v>0.89</v>
@@ -19463,25 +19397,22 @@
       <c r="AP23">
         <v>0</v>
       </c>
-      <c r="AQ23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F24">
         <v>0.92</v>
@@ -19594,25 +19525,22 @@
       <c r="AP24">
         <v>0</v>
       </c>
-      <c r="AQ24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F25" s="17">
         <v>0.92</v>
@@ -19725,12 +19653,9 @@
       <c r="AP25" s="17">
         <v>0</v>
       </c>
-      <c r="AQ25" s="17">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AQ25">
+  <conditionalFormatting sqref="B3:AP25">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -19743,7 +19668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062F9C9F-EC6B-45A0-B400-3E864B701D31}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
@@ -19754,13 +19679,13 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D1" t="s">
         <v>196</v>
@@ -19784,28 +19709,28 @@
         <v>153</v>
       </c>
       <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
         <v>250</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>251</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>252</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>253</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>254</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>255</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>256</v>
-      </c>
-      <c r="R1" t="s">
-        <v>257</v>
       </c>
       <c r="S1" t="s">
         <v>190</v>
@@ -19820,30 +19745,30 @@
         <v>194</v>
       </c>
       <c r="W1" t="s">
+        <v>257</v>
+      </c>
+      <c r="X1" t="s">
         <v>258</v>
-      </c>
-      <c r="X1" t="s">
-        <v>259</v>
       </c>
       <c r="Y1" t="s">
         <v>200</v>
       </c>
       <c r="Z1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AA1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>261</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>262</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -19915,18 +19840,18 @@
         <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -20003,13 +19928,13 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -20086,13 +20011,13 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -20164,18 +20089,18 @@
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -20247,18 +20172,18 @@
         <v>0</v>
       </c>
       <c r="AA7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -20330,7 +20255,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -20358,13 +20283,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D1" t="s">
         <v>188</v>
@@ -20402,13 +20327,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>270</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>271</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -20446,13 +20371,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -20490,13 +20415,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -20534,13 +20459,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -20578,13 +20503,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -20622,13 +20547,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -20666,13 +20591,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -20710,13 +20635,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D10">
         <v>0.9</v>
@@ -20754,13 +20679,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -20798,13 +20723,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -20842,13 +20767,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -20886,13 +20811,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -20930,13 +20855,13 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -20974,13 +20899,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -21018,13 +20943,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -21062,13 +20987,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -21106,13 +21031,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -21150,13 +21075,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D20">
         <v>1</v>

</xml_diff>

<commit_message>
code(US-Tool): move the heat extraction to the us-sheet, since this is a location-dependent variable.
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129BF5FB-302D-D04B-A26F-FD7329CBCC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1587C9C1-E11B-C441-8B29-5F65B9248494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34520" yWindow="500" windowWidth="34280" windowHeight="26300" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="360">
   <si>
     <t>start date</t>
   </si>
@@ -653,9 +653,6 @@
   </si>
   <si>
     <t>quality grade</t>
-  </si>
-  <si>
-    <t>heat extraction</t>
   </si>
   <si>
     <t>min. borehole area</t>
@@ -1750,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1765,7 +1762,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1802,7 +1799,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -1828,13 +1825,13 @@
         <v>105</v>
       </c>
       <c r="B1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" t="s">
         <v>279</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>280</v>
-      </c>
-      <c r="D1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3351,7 +3348,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B111">
         <v>0.35</v>
@@ -3365,7 +3362,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B112">
         <v>0.21</v>
@@ -3393,7 +3390,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B114">
         <v>7.14</v>
@@ -3421,7 +3418,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B116">
         <v>286</v>
@@ -3466,19 +3463,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>289</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>197</v>
@@ -3499,13 +3496,13 @@
         <v>153</v>
       </c>
       <c r="L1" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>291</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>292</v>
       </c>
       <c r="O1" t="s">
         <v>188</v>
@@ -3529,7 +3526,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" s="13">
         <v>0</v>
@@ -3562,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M3" s="13">
         <v>1</v>
@@ -3576,7 +3573,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B4" s="13">
         <v>0</v>
@@ -3609,7 +3606,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M4" s="13">
         <v>1</v>
@@ -3623,7 +3620,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B5" s="13">
         <v>0</v>
@@ -3656,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M5" s="13">
         <v>1</v>
@@ -3670,7 +3667,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
@@ -3703,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M6" s="13">
         <v>1</v>
@@ -3717,7 +3714,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -3750,7 +3747,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M7" s="13">
         <v>1</v>
@@ -3764,7 +3761,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
@@ -3797,7 +3794,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M8" s="13">
         <v>0</v>
@@ -3811,7 +3808,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
@@ -3844,7 +3841,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M9" s="13">
         <v>1</v>
@@ -3858,7 +3855,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B10" s="13">
         <v>0</v>
@@ -3891,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M10" s="13">
         <v>1</v>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B11" s="13">
         <v>0</v>
@@ -3938,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M11" s="13">
         <v>1</v>
@@ -3952,7 +3949,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" s="13">
         <v>0</v>
@@ -3985,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M12" s="13">
         <v>1</v>
@@ -3999,7 +3996,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B13" s="13">
         <v>0</v>
@@ -4032,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M13" s="13">
         <v>1</v>
@@ -4046,7 +4043,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B14" s="13">
         <v>0</v>
@@ -4079,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M14" s="13">
         <v>1</v>
@@ -4093,7 +4090,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B15" s="13">
         <v>0</v>
@@ -4126,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M15" s="13">
         <v>1</v>
@@ -4140,7 +4137,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
@@ -4173,7 +4170,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M16" s="13">
         <v>1</v>
@@ -4187,7 +4184,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
@@ -4220,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M17" s="13">
         <v>1</v>
@@ -4234,7 +4231,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B18" s="13">
         <v>0</v>
@@ -4267,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M18" s="13">
         <v>1</v>
@@ -4281,7 +4278,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B19" s="13">
         <v>0</v>
@@ -4314,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M19" s="13">
         <v>1</v>
@@ -4328,7 +4325,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B20" s="13">
         <v>0</v>
@@ -4361,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M20" s="13">
         <v>1</v>
@@ -4375,7 +4372,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B21" s="13">
         <v>0</v>
@@ -4408,7 +4405,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M21" s="13">
         <v>1</v>
@@ -4422,7 +4419,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B22" s="13">
         <v>0</v>
@@ -4455,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M22" s="13">
         <v>1</v>
@@ -4469,7 +4466,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4502,7 +4499,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -4516,7 +4513,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4563,7 +4560,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4610,7 +4607,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4686,13 +4683,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>188</v>
@@ -4706,7 +4703,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B2" s="6">
         <v>0.15655827580000001</v>
@@ -4726,7 +4723,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B3" s="6">
         <v>85</v>
@@ -4746,7 +4743,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4808,7 +4805,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4837,7 +4834,7 @@
         <v>366</v>
       </c>
       <c r="I3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4866,7 +4863,7 @@
         <v>366</v>
       </c>
       <c r="I4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4895,7 +4892,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5069,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5098,7 +5095,7 @@
         <v>366</v>
       </c>
       <c r="I12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5185,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5214,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5243,7 +5240,7 @@
         <v>366</v>
       </c>
       <c r="I17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -5272,7 +5269,7 @@
         <v>366</v>
       </c>
       <c r="I18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -5301,7 +5298,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -5330,7 +5327,7 @@
         <v>436</v>
       </c>
       <c r="I20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -5359,7 +5356,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -5393,7 +5390,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5417,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -5475,7 +5472,7 @@
         <v>366</v>
       </c>
       <c r="I25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -5509,7 +5506,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -5533,7 +5530,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -5562,7 +5559,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -5620,7 +5617,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -5678,7 +5675,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -5799,7 +5796,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -5885,7 +5882,7 @@
         <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -5920,7 +5917,7 @@
         <v>0.9</v>
       </c>
       <c r="J3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -5952,7 +5949,7 @@
         <v>0.9</v>
       </c>
       <c r="J4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -5984,7 +5981,7 @@
         <v>0.9</v>
       </c>
       <c r="J5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -6016,7 +6013,7 @@
         <v>0.9</v>
       </c>
       <c r="J6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -6048,7 +6045,7 @@
         <v>0.9</v>
       </c>
       <c r="J7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -6080,7 +6077,7 @@
         <v>0.9</v>
       </c>
       <c r="J8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6112,7 +6109,7 @@
         <v>0.9</v>
       </c>
       <c r="J9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -6144,7 +6141,7 @@
         <v>0.9</v>
       </c>
       <c r="J10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -6176,7 +6173,7 @@
         <v>0.85</v>
       </c>
       <c r="J11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -6208,7 +6205,7 @@
         <v>0.85</v>
       </c>
       <c r="J12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -6240,7 +6237,7 @@
         <v>0.89</v>
       </c>
       <c r="J13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -6272,7 +6269,7 @@
         <v>0.89</v>
       </c>
       <c r="J14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -6304,7 +6301,7 @@
         <v>0.9</v>
       </c>
       <c r="J15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -6336,7 +6333,7 @@
         <v>0.9</v>
       </c>
       <c r="J16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -6368,7 +6365,7 @@
         <v>0.91</v>
       </c>
       <c r="J17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -6400,7 +6397,7 @@
         <v>0.91</v>
       </c>
       <c r="J18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -6432,7 +6429,7 @@
         <v>0.91</v>
       </c>
       <c r="J19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -6464,7 +6461,7 @@
         <v>0.91</v>
       </c>
       <c r="J20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -6496,7 +6493,7 @@
         <v>0.9</v>
       </c>
       <c r="J21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -6528,7 +6525,7 @@
         <v>0.9</v>
       </c>
       <c r="J22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -6560,7 +6557,7 @@
         <v>0.9</v>
       </c>
       <c r="J23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6592,7 +6589,7 @@
         <v>0.9</v>
       </c>
       <c r="J24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -6624,7 +6621,7 @@
         <v>0.9</v>
       </c>
       <c r="J25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -6656,7 +6653,7 @@
         <v>0.9</v>
       </c>
       <c r="J26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -6688,7 +6685,7 @@
         <v>0.85</v>
       </c>
       <c r="J27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -6720,7 +6717,7 @@
         <v>0.85</v>
       </c>
       <c r="J28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -6752,7 +6749,7 @@
         <v>0.91</v>
       </c>
       <c r="J29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -6784,7 +6781,7 @@
         <v>0.91</v>
       </c>
       <c r="J30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -6816,7 +6813,7 @@
         <v>0.91</v>
       </c>
       <c r="J31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -6848,7 +6845,7 @@
         <v>0.91</v>
       </c>
       <c r="J32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -6880,7 +6877,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -15962,7 +15959,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -16058,7 +16055,7 @@
         <v>196</v>
       </c>
       <c r="AG1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -16164,7 +16161,7 @@
         <v>0</v>
       </c>
       <c r="AG3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
@@ -16265,7 +16262,7 @@
         <v>0</v>
       </c>
       <c r="AG4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -16366,7 +16363,7 @@
         <v>0</v>
       </c>
       <c r="AG5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
@@ -16467,7 +16464,7 @@
         <v>0</v>
       </c>
       <c r="AG6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -16568,7 +16565,7 @@
         <v>0</v>
       </c>
       <c r="AG7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -16583,10 +16580,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
-  <dimension ref="A1:AP25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16597,15 +16594,15 @@
     <col min="12" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D1" t="s">
         <v>147</v>
@@ -16721,25 +16718,22 @@
       <c r="AO1" t="s">
         <v>218</v>
       </c>
-      <c r="AP1" t="s">
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E3" t="s">
         <v>220</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E3" t="s">
-        <v>221</v>
       </c>
       <c r="F3">
         <v>0.375</v>
@@ -16849,25 +16843,22 @@
       <c r="AO3">
         <v>0</v>
       </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F4">
         <v>0.39</v>
@@ -16977,25 +16968,22 @@
       <c r="AO4">
         <v>0</v>
       </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F5">
         <v>0.92</v>
@@ -17105,25 +17093,22 @@
       <c r="AO5">
         <v>0</v>
       </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" t="s">
+        <v>347</v>
+      </c>
+      <c r="E6" t="s">
         <v>224</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>339</v>
-      </c>
-      <c r="D6" t="s">
-        <v>348</v>
-      </c>
-      <c r="E6" t="s">
-        <v>225</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -17171,10 +17156,10 @@
         <v>0</v>
       </c>
       <c r="U6" t="s">
+        <v>225</v>
+      </c>
+      <c r="V6" t="s">
         <v>226</v>
-      </c>
-      <c r="V6" t="s">
-        <v>227</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -17183,10 +17168,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="Y6">
-        <v>3.2800000000000003E-2</v>
+        <v>100</v>
       </c>
       <c r="Z6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -17233,25 +17218,22 @@
       <c r="AO6">
         <v>0</v>
       </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -17299,10 +17281,10 @@
         <v>0</v>
       </c>
       <c r="U7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -17314,13 +17296,13 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA7">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AB7">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -17361,25 +17343,22 @@
       <c r="AO7">
         <v>0</v>
       </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -17427,10 +17406,10 @@
         <v>0</v>
       </c>
       <c r="U8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -17489,25 +17468,22 @@
       <c r="AO8">
         <v>0</v>
       </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -17555,10 +17531,10 @@
         <v>0</v>
       </c>
       <c r="U9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -17570,13 +17546,13 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA9">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="AB9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -17617,25 +17593,22 @@
       <c r="AO9">
         <v>0</v>
       </c>
-      <c r="AP9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" t="s">
         <v>351</v>
       </c>
-      <c r="D10" t="s">
-        <v>352</v>
-      </c>
       <c r="E10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -17745,13 +17718,10 @@
       <c r="AO10">
         <v>0</v>
       </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -17760,7 +17730,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F11">
         <v>0.78500000000000003</v>
@@ -17870,13 +17840,10 @@
       <c r="AO11">
         <v>0</v>
       </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -17885,7 +17852,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F12">
         <v>0.83</v>
@@ -17995,25 +17962,22 @@
       <c r="AO12">
         <v>0</v>
       </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F13">
         <v>0.4</v>
@@ -18123,13 +18087,10 @@
       <c r="AO13">
         <v>0</v>
       </c>
-      <c r="AP13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -18138,7 +18099,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F14">
         <v>0.98</v>
@@ -18248,13 +18209,10 @@
       <c r="AO14">
         <v>0</v>
       </c>
-      <c r="AP14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -18263,7 +18221,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F15">
         <v>0.98</v>
@@ -18373,13 +18331,10 @@
       <c r="AO15">
         <v>0</v>
       </c>
-      <c r="AP15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -18388,7 +18343,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F16">
         <v>0.98</v>
@@ -18498,25 +18453,22 @@
       <c r="AO16">
         <v>0</v>
       </c>
-      <c r="AP16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F17">
         <v>0.92</v>
@@ -18626,25 +18578,22 @@
       <c r="AO17">
         <v>0</v>
       </c>
-      <c r="AP17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -18692,10 +18641,10 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
+        <v>225</v>
+      </c>
+      <c r="V18" t="s">
         <v>226</v>
-      </c>
-      <c r="V18" t="s">
-        <v>227</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -18704,10 +18653,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="Y18">
-        <v>3.2800000000000003E-2</v>
+        <v>100</v>
       </c>
       <c r="Z18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA18">
         <v>0</v>
@@ -18754,25 +18703,22 @@
       <c r="AO18">
         <v>0</v>
       </c>
-      <c r="AP18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F19">
         <v>0.35</v>
@@ -18882,25 +18828,22 @@
       <c r="AO19">
         <v>0</v>
       </c>
-      <c r="AP19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F20">
         <v>0.35</v>
@@ -19010,25 +18953,22 @@
       <c r="AO20">
         <v>0</v>
       </c>
-      <c r="AP20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F21">
         <v>0.92</v>
@@ -19138,25 +19078,22 @@
       <c r="AO21">
         <v>0</v>
       </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F22">
         <v>0.9</v>
@@ -19266,25 +19203,22 @@
       <c r="AO22">
         <v>0</v>
       </c>
-      <c r="AP22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F23">
         <v>0.89</v>
@@ -19394,25 +19328,22 @@
       <c r="AO23">
         <v>0</v>
       </c>
-      <c r="AP23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F24">
         <v>0.92</v>
@@ -19522,25 +19453,22 @@
       <c r="AO24">
         <v>0</v>
       </c>
-      <c r="AP24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F25" s="17">
         <v>0.92</v>
@@ -19650,12 +19578,9 @@
       <c r="AO25" s="17">
         <v>0</v>
       </c>
-      <c r="AP25" s="17">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AP25">
+  <conditionalFormatting sqref="B3:AO25">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -19679,13 +19604,13 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D1" t="s">
         <v>196</v>
@@ -19709,28 +19634,28 @@
         <v>153</v>
       </c>
       <c r="K1" t="s">
+        <v>248</v>
+      </c>
+      <c r="L1" t="s">
         <v>249</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>250</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>251</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>252</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>253</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>254</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>255</v>
-      </c>
-      <c r="R1" t="s">
-        <v>256</v>
       </c>
       <c r="S1" t="s">
         <v>190</v>
@@ -19745,30 +19670,30 @@
         <v>194</v>
       </c>
       <c r="W1" t="s">
+        <v>256</v>
+      </c>
+      <c r="X1" t="s">
         <v>257</v>
-      </c>
-      <c r="X1" t="s">
-        <v>258</v>
       </c>
       <c r="Y1" t="s">
         <v>200</v>
       </c>
       <c r="Z1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AA1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>260</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>261</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -19840,18 +19765,18 @@
         <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -19928,13 +19853,13 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -20011,13 +19936,13 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -20089,18 +20014,18 @@
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -20172,18 +20097,18 @@
         <v>0</v>
       </c>
       <c r="AA7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -20255,7 +20180,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -20283,13 +20208,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" t="s">
         <v>188</v>
@@ -20327,13 +20252,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>269</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>270</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -20371,13 +20296,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -20415,13 +20340,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -20459,13 +20384,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -20503,13 +20428,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -20547,13 +20472,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -20591,13 +20516,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -20635,13 +20560,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D10">
         <v>0.9</v>
@@ -20679,13 +20604,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -20723,13 +20648,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -20767,13 +20692,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -20811,13 +20736,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -20855,13 +20780,13 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -20899,13 +20824,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -20943,13 +20868,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -20987,13 +20912,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -21031,13 +20956,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -21075,13 +21000,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D20">
         <v>1</v>

</xml_diff>

<commit_message>
code(US-Tool): Implementation of the division of the sink for wood stove and St in order to represent their heat share correctly in the status quo.
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1587C9C1-E11B-C441-8B29-5F65B9248494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EB63A6-1BC0-4846-936E-EE184E218E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34520" yWindow="500" windowWidth="34280" windowHeight="26300" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="7" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="361">
   <si>
     <t>start date</t>
   </si>
@@ -1127,6 +1127,9 @@
   </si>
   <si>
     <t>stove_heating</t>
+  </si>
+  <si>
+    <t>heat_share_link</t>
   </si>
 </sst>
 </file>
@@ -16582,7 +16585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
   <dimension ref="A1:AO25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
@@ -19593,8 +19596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062F9C9F-EC6B-45A0-B400-3E864B701D31}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19732,7 +19735,7 @@
         <v>0.98</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q3">
         <v>0.1</v>
@@ -19981,7 +19984,7 @@
         <v>0.98</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q6">
         <v>0.1</v>
@@ -20195,10 +20198,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F7A117-64AB-4955-A232-50A2E399D809}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21042,8 +21045,52 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>269</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>9999</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K21">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:N18">
+  <conditionalFormatting sqref="A3:N18 A21:N21">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
code(US-Tool): add building pellet transformer
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EB63A6-1BC0-4846-936E-EE184E218E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF26F596-7172-FA45-9800-5FA1F4185502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="7" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18740" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="363">
   <si>
     <t>start date</t>
   </si>
@@ -1130,6 +1130,12 @@
   </si>
   <si>
     <t>heat_share_link</t>
+  </si>
+  <si>
+    <t>building_pelletheating_transformer</t>
+  </si>
+  <si>
+    <t>building_pellet_bus</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1322,14 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3435,7 +3448,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4657,7 +4670,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4771,10 +4784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5826,14 +5839,43 @@
         <v>10</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>362</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="17">
+        <v>100</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3:H22">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6 B24:H37">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+  <conditionalFormatting sqref="F6 B24:H38">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6885,7 +6927,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I26 B31:I32">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15706,7 +15748,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z110">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15936,7 +15978,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:W3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16573,7 +16615,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AF7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16583,10 +16625,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
-  <dimension ref="A1:AO25"/>
+  <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19582,9 +19624,139 @@
         <v>0</v>
       </c>
     </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>361</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>338</v>
+      </c>
+      <c r="D26" t="s">
+        <v>356</v>
+      </c>
+      <c r="E26" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.92</v>
+      </c>
+      <c r="G26" s="17">
+        <v>0</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17">
+        <v>0</v>
+      </c>
+      <c r="L26" s="17">
+        <v>317</v>
+      </c>
+      <c r="M26" s="17">
+        <v>0</v>
+      </c>
+      <c r="N26" s="17">
+        <v>0</v>
+      </c>
+      <c r="O26" s="17">
+        <v>500</v>
+      </c>
+      <c r="P26" s="17">
+        <v>75</v>
+      </c>
+      <c r="Q26" s="17">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R26" s="17">
+        <v>0</v>
+      </c>
+      <c r="S26" s="17">
+        <v>0</v>
+      </c>
+      <c r="T26" s="17">
+        <v>0</v>
+      </c>
+      <c r="U26" s="17">
+        <v>0</v>
+      </c>
+      <c r="V26" s="17">
+        <v>0</v>
+      </c>
+      <c r="W26" s="17">
+        <v>0</v>
+      </c>
+      <c r="X26" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AO25">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:AO26">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19596,7 +19768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062F9C9F-EC6B-45A0-B400-3E864B701D31}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
@@ -20188,7 +20360,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21091,17 +21263,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:N18 A21:N21">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:N20">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:N19">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
code( ): add new technology AAHP to the SESMG algorithm as well as the US Tool
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF26F596-7172-FA45-9800-5FA1F4185502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75373CEE-A081-EA48-AB59-7269285FC0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18740" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18740" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="366">
   <si>
     <t>start date</t>
   </si>
@@ -1136,6 +1136,15 @@
   </si>
   <si>
     <t>building_pellet_bus</t>
+  </si>
+  <si>
+    <t>building_aahp_transformer</t>
+  </si>
+  <si>
+    <t>AAHP</t>
+  </si>
+  <si>
+    <t>Air-to-Air</t>
   </si>
 </sst>
 </file>
@@ -1319,17 +1328,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -1435,7 +1437,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3448,7 +3450,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4670,7 +4672,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4786,7 +4788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -5870,12 +5872,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:H22">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6 B24:H38">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6927,7 +6929,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I26 B31:I32">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15748,7 +15750,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z110">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15978,7 +15980,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:W3">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16615,7 +16617,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AF7">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16625,10 +16627,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
-  <dimension ref="A1:AO26"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AP27" sqref="AP27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19548,7 +19550,7 @@
       <c r="P25" s="17">
         <v>75</v>
       </c>
-      <c r="Q25" s="17">
+      <c r="Q25">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="R25" s="17">
@@ -19673,7 +19675,7 @@
       <c r="P26" s="17">
         <v>75</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="R26" s="17">
@@ -19749,14 +19751,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>363</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>338</v>
+      </c>
+      <c r="D27" t="s">
+        <v>364</v>
+      </c>
+      <c r="E27" t="s">
+        <v>224</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="17">
+        <v>100</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>500</v>
+      </c>
+      <c r="P27" s="17">
+        <v>100</v>
+      </c>
+      <c r="Q27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>225</v>
+      </c>
+      <c r="V27" t="s">
+        <v>365</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AO25">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:AO26">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="B3:AO26 B27:T27 W27:AO27">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20360,7 +20482,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z8">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21262,18 +21384,18 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:N18 A21:N21">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="A3:N18">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:N20">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="A20:N21">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:N19">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
documentation(US-Tool): update source code structure and documentation
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75373CEE-A081-EA48-AB59-7269285FC0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F399CE9F-753C-AC45-A0FA-EFB18FFB5A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18740" activeTab="6" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="31760" yWindow="500" windowWidth="33600" windowHeight="18740" activeTab="8" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="368">
   <si>
     <t>start date</t>
   </si>
@@ -1145,6 +1145,12 @@
   </si>
   <si>
     <t>Air-to-Air</t>
+  </si>
+  <si>
+    <t>central_electricity_shortage_bus</t>
+  </si>
+  <si>
+    <t>central_pv_central_link</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1334,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
   <dxfs count="13">
@@ -1437,9 +1443,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1477,7 +1483,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1583,7 +1589,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1725,7 +1731,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4786,10 +4792,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5321,7 +5327,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>366</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5330,33 +5336,33 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1.4999999999999999E-2</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>436</v>
+        <v>100</v>
       </c>
       <c r="I20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -5365,13 +5371,13 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>436</v>
       </c>
       <c r="I21" t="s">
         <v>338</v>
@@ -5379,71 +5385,71 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0.15620000000000001</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>10</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>333</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.15620000000000001</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="I23" t="s">
-        <v>338</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>333</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -5461,12 +5467,12 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>10</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5475,27 +5481,27 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0.1958</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>366</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>337</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5510,50 +5516,50 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>4.4999999999999998E-2</v>
+        <v>0.1958</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="I26" t="s">
-        <v>10</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>320</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>-0.1215</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G27">
-        <v>-1.39</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>337</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>320</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -5565,13 +5571,13 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>-5.1459999999999999E-2</v>
+        <v>-0.1215</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>-27</v>
+        <v>-1.39</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -5582,152 +5588,152 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>-5.1459999999999999E-2</v>
       </c>
       <c r="F29">
-        <v>9.4500000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>-27</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>10</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="G30">
-        <v>-95</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>337</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F31">
-        <v>2.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>-95</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>10</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G32">
-        <v>-95</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>337</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F33">
-        <v>4.4999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>-95</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>10</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5742,7 +5748,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>9.7000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -5756,7 +5762,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5771,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>9.4500000000000001E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -5785,7 +5791,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -5800,7 +5806,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>2.9000000000000001E-2</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -5814,7 +5820,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>335</v>
+        <v>50</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -5828,8 +5834,8 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37" s="17">
-        <v>100</v>
+      <c r="F37">
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -5843,7 +5849,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -5870,13 +5876,42 @@
         <v>10</v>
       </c>
     </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>362</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="17">
+        <v>100</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:H22">
+  <conditionalFormatting sqref="B3:H23">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6 B24:H38">
+  <conditionalFormatting sqref="F6 B25:H39">
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -16629,7 +16664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
   <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AP27" sqref="AP27"/>
     </sheetView>
   </sheetViews>
@@ -20492,10 +20527,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F7A117-64AB-4955-A232-50A2E399D809}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20857,7 +20892,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>367</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -20866,7 +20901,7 @@
         <v>269</v>
       </c>
       <c r="D10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -20901,7 +20936,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -20910,7 +20945,7 @@
         <v>269</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -20945,7 +20980,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -20989,7 +21024,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -21033,7 +21068,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -21077,7 +21112,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -21121,7 +21156,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -21165,7 +21200,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -21209,7 +21244,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -21253,7 +21288,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -21297,7 +21332,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -21341,7 +21376,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -21383,18 +21418,62 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>360</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>269</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>9999</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K22">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:N18">
+  <conditionalFormatting sqref="A3:N19">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:N21">
+  <conditionalFormatting sqref="A21:N22">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:N19">
+  <conditionalFormatting sqref="B20:N20">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
documentation( ): update comments in code and bug fixes
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters_example.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F399CE9F-753C-AC45-A0FA-EFB18FFB5A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5687A3-40D7-9845-AD45-26DD194192A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31760" yWindow="500" windowWidth="33600" windowHeight="18740" activeTab="8" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="369">
   <si>
     <t>start date</t>
   </si>
@@ -1009,9 +1009,6 @@
     <t>anergy_heat_pump</t>
   </si>
   <si>
-    <t>screw_turbine_bus</t>
-  </si>
-  <si>
     <t>source_type</t>
   </si>
   <si>
@@ -1151,6 +1148,12 @@
   </si>
   <si>
     <t>central_pv_central_link</t>
+  </si>
+  <si>
+    <t>central_timeseries_source_bus</t>
+  </si>
+  <si>
+    <t>central_timeseries_central_link</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1340,14 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1771,7 +1781,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1786,7 +1796,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1823,7 +1833,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3456,7 +3466,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4678,7 +4688,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4795,7 +4805,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4829,7 +4839,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4858,7 +4868,7 @@
         <v>366</v>
       </c>
       <c r="I3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4887,7 +4897,7 @@
         <v>366</v>
       </c>
       <c r="I4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4916,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5090,7 +5100,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5119,7 +5129,7 @@
         <v>366</v>
       </c>
       <c r="I12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5206,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5235,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5264,7 +5274,7 @@
         <v>366</v>
       </c>
       <c r="I17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -5293,7 +5303,7 @@
         <v>366</v>
       </c>
       <c r="I18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -5322,12 +5332,12 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5351,7 +5361,7 @@
         <v>100</v>
       </c>
       <c r="I20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -5380,7 +5390,7 @@
         <v>436</v>
       </c>
       <c r="I21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -5409,7 +5419,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -5443,7 +5453,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5467,7 +5477,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -5525,7 +5535,7 @@
         <v>366</v>
       </c>
       <c r="I26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -5559,7 +5569,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>320</v>
+        <v>367</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -5583,7 +5593,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -5612,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -5670,7 +5680,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5728,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -5849,7 +5859,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -5878,7 +5888,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -5907,12 +5917,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:H23">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6 B25:H39">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5964,7 +5974,7 @@
         <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -5999,7 +6009,7 @@
         <v>0.9</v>
       </c>
       <c r="J3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -6031,7 +6041,7 @@
         <v>0.9</v>
       </c>
       <c r="J4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -6063,7 +6073,7 @@
         <v>0.9</v>
       </c>
       <c r="J5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -6095,7 +6105,7 @@
         <v>0.9</v>
       </c>
       <c r="J6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -6127,7 +6137,7 @@
         <v>0.9</v>
       </c>
       <c r="J7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -6159,7 +6169,7 @@
         <v>0.9</v>
       </c>
       <c r="J8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6191,7 +6201,7 @@
         <v>0.9</v>
       </c>
       <c r="J9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -6223,7 +6233,7 @@
         <v>0.9</v>
       </c>
       <c r="J10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -6255,7 +6265,7 @@
         <v>0.85</v>
       </c>
       <c r="J11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -6287,7 +6297,7 @@
         <v>0.85</v>
       </c>
       <c r="J12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -6319,7 +6329,7 @@
         <v>0.89</v>
       </c>
       <c r="J13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -6351,7 +6361,7 @@
         <v>0.89</v>
       </c>
       <c r="J14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -6383,7 +6393,7 @@
         <v>0.9</v>
       </c>
       <c r="J15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -6415,7 +6425,7 @@
         <v>0.9</v>
       </c>
       <c r="J16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -6447,7 +6457,7 @@
         <v>0.91</v>
       </c>
       <c r="J17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -6479,7 +6489,7 @@
         <v>0.91</v>
       </c>
       <c r="J18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -6511,7 +6521,7 @@
         <v>0.91</v>
       </c>
       <c r="J19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -6543,7 +6553,7 @@
         <v>0.91</v>
       </c>
       <c r="J20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -6575,7 +6585,7 @@
         <v>0.9</v>
       </c>
       <c r="J21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -6607,7 +6617,7 @@
         <v>0.9</v>
       </c>
       <c r="J22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -6639,7 +6649,7 @@
         <v>0.9</v>
       </c>
       <c r="J23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6671,7 +6681,7 @@
         <v>0.9</v>
       </c>
       <c r="J24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -6703,7 +6713,7 @@
         <v>0.9</v>
       </c>
       <c r="J25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -6735,7 +6745,7 @@
         <v>0.9</v>
       </c>
       <c r="J26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -6767,7 +6777,7 @@
         <v>0.85</v>
       </c>
       <c r="J27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -6799,7 +6809,7 @@
         <v>0.85</v>
       </c>
       <c r="J28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -6831,7 +6841,7 @@
         <v>0.91</v>
       </c>
       <c r="J29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -6863,7 +6873,7 @@
         <v>0.91</v>
       </c>
       <c r="J30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -6895,7 +6905,7 @@
         <v>0.91</v>
       </c>
       <c r="J31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -6927,7 +6937,7 @@
         <v>0.91</v>
       </c>
       <c r="J32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -6959,12 +6969,12 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I26 B31:I32">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15785,7 +15795,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z110">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16015,7 +16025,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:W3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16041,7 +16051,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -16137,7 +16147,7 @@
         <v>196</v>
       </c>
       <c r="AG1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -16243,7 +16253,7 @@
         <v>0</v>
       </c>
       <c r="AG3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
@@ -16344,7 +16354,7 @@
         <v>0</v>
       </c>
       <c r="AG4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -16445,7 +16455,7 @@
         <v>0</v>
       </c>
       <c r="AG5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
@@ -16546,7 +16556,7 @@
         <v>0</v>
       </c>
       <c r="AG6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -16647,12 +16657,12 @@
         <v>0</v>
       </c>
       <c r="AG7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AF7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16678,13 +16688,13 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D1" t="s">
         <v>147</v>
@@ -16809,10 +16819,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E3" t="s">
         <v>220</v>
@@ -16934,10 +16944,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E4" t="s">
         <v>220</v>
@@ -17059,10 +17069,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5" t="s">
         <v>220</v>
@@ -17184,10 +17194,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E6" t="s">
         <v>224</v>
@@ -17309,10 +17319,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E7" t="s">
         <v>224</v>
@@ -17434,10 +17444,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E8" t="s">
         <v>224</v>
@@ -17559,10 +17569,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E9" t="s">
         <v>224</v>
@@ -17684,10 +17694,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D10" t="s">
         <v>350</v>
-      </c>
-      <c r="D10" t="s">
-        <v>351</v>
       </c>
       <c r="E10" t="s">
         <v>220</v>
@@ -18053,10 +18063,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E13" t="s">
         <v>220</v>
@@ -18544,10 +18554,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E17" t="s">
         <v>220</v>
@@ -18669,10 +18679,10 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E18" t="s">
         <v>224</v>
@@ -18794,10 +18804,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E19" t="s">
         <v>220</v>
@@ -18919,10 +18929,10 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E20" t="s">
         <v>220</v>
@@ -19044,10 +19054,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E21" t="s">
         <v>220</v>
@@ -19169,10 +19179,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E22" t="s">
         <v>220</v>
@@ -19294,10 +19304,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D23" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E23" t="s">
         <v>220</v>
@@ -19419,10 +19429,10 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E24" t="s">
         <v>220</v>
@@ -19538,16 +19548,16 @@
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E25" t="s">
         <v>220</v>
@@ -19663,16 +19673,16 @@
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E26" t="s">
         <v>220</v>
@@ -19788,16 +19798,16 @@
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>362</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>337</v>
+      </c>
+      <c r="D27" t="s">
         <v>363</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>338</v>
-      </c>
-      <c r="D27" t="s">
-        <v>364</v>
       </c>
       <c r="E27" t="s">
         <v>224</v>
@@ -19851,7 +19861,7 @@
         <v>225</v>
       </c>
       <c r="V27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -19913,7 +19923,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AO26 B27:T27 W27:AO27">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19936,7 +19946,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -20014,7 +20024,7 @@
         <v>258</v>
       </c>
       <c r="AA1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -20097,7 +20107,7 @@
         <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -20346,7 +20356,7 @@
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
@@ -20429,7 +20439,7 @@
         <v>0</v>
       </c>
       <c r="AA7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -20512,12 +20522,12 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20527,10 +20537,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F7A117-64AB-4955-A232-50A2E399D809}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B23" sqref="B23:N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20628,7 +20638,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -20892,7 +20902,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -21068,7 +21078,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -21112,7 +21122,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -21156,7 +21166,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -21200,7 +21210,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -21244,7 +21254,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -21288,7 +21298,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -21332,7 +21342,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -21376,7 +21386,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -21420,7 +21430,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -21462,19 +21472,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>269</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>9999</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K23">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A3:N19">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:N22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="A21:N22 A23">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:N20">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:N23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>